<commit_message>
Correction minor error in mapping.
</commit_message>
<xml_diff>
--- a/src/Data/eco3.6_exio3/Product_Concordances.xlsx
+++ b/src/Data/eco3.6_exio3/Product_Concordances.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maxime\Desktop\Thesis\Modules_Python\pylcaio\src\Data\eco3.6_exio3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{768769FA-62A5-4EC7-A77B-EE5B2A4A0536}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C863D1BC-C5C8-4D64-95D4-20C1D2BA7C0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22224" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="22224" windowHeight="13176" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Description_Exiobase" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8822" uniqueCount="6011">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8819" uniqueCount="6011">
   <si>
     <t>ProductTypeName</t>
   </si>
@@ -18575,7 +18575,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C202"/>
   <sheetViews>
-    <sheetView topLeftCell="A146" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A122" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="A163" sqref="A163"/>
     </sheetView>
   </sheetViews>
@@ -20412,7 +20412,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C2300"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2196" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G2215" sqref="G2215"/>
     </sheetView>
@@ -45733,10 +45733,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A481ADA-D006-4410-B77F-025CE597EEA8}">
-  <dimension ref="A1:C506"/>
+  <dimension ref="A1:C505"/>
   <sheetViews>
-    <sheetView topLeftCell="A488" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B519" sqref="B519"/>
+    <sheetView tabSelected="1" topLeftCell="A344" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E363" sqref="E363"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -49757,26 +49757,26 @@
         <v>1711</v>
       </c>
       <c r="C365" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
     </row>
     <row r="366" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A366" t="s">
-        <v>5596</v>
+        <v>5597</v>
       </c>
       <c r="B366" t="s">
-        <v>1712</v>
+        <v>881</v>
       </c>
       <c r="C366" t="s">
-        <v>253</v>
+        <v>234</v>
       </c>
     </row>
     <row r="367" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A367" t="s">
-        <v>5597</v>
+        <v>5598</v>
       </c>
       <c r="B367" t="s">
-        <v>881</v>
+        <v>754</v>
       </c>
       <c r="C367" t="s">
         <v>234</v>
@@ -49784,10 +49784,10 @@
     </row>
     <row r="368" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A368" t="s">
-        <v>5598</v>
+        <v>5599</v>
       </c>
       <c r="B368" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
       <c r="C368" t="s">
         <v>234</v>
@@ -49795,32 +49795,32 @@
     </row>
     <row r="369" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A369" t="s">
-        <v>5599</v>
+        <v>5600</v>
       </c>
       <c r="B369" t="s">
-        <v>755</v>
+        <v>886</v>
       </c>
       <c r="C369" t="s">
-        <v>234</v>
+        <v>253</v>
       </c>
     </row>
     <row r="370" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A370" t="s">
-        <v>5600</v>
+        <v>5601</v>
       </c>
       <c r="B370" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="C370" t="s">
-        <v>253</v>
+        <v>234</v>
       </c>
     </row>
     <row r="371" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A371" t="s">
-        <v>5601</v>
+        <v>5602</v>
       </c>
       <c r="B371" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="C371" t="s">
         <v>234</v>
@@ -49828,10 +49828,10 @@
     </row>
     <row r="372" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A372" t="s">
-        <v>5602</v>
+        <v>5603</v>
       </c>
       <c r="B372" t="s">
-        <v>888</v>
+        <v>883</v>
       </c>
       <c r="C372" t="s">
         <v>234</v>
@@ -49839,10 +49839,10 @@
     </row>
     <row r="373" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A373" t="s">
-        <v>5603</v>
+        <v>5604</v>
       </c>
       <c r="B373" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="C373" t="s">
         <v>234</v>
@@ -49850,10 +49850,10 @@
     </row>
     <row r="374" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A374" t="s">
-        <v>5604</v>
+        <v>5605</v>
       </c>
       <c r="B374" t="s">
-        <v>882</v>
+        <v>884</v>
       </c>
       <c r="C374" t="s">
         <v>234</v>
@@ -49861,21 +49861,21 @@
     </row>
     <row r="375" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A375" t="s">
-        <v>5605</v>
+        <v>5606</v>
       </c>
       <c r="B375" t="s">
-        <v>884</v>
+        <v>1713</v>
       </c>
       <c r="C375" t="s">
-        <v>234</v>
+        <v>253</v>
       </c>
     </row>
     <row r="376" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A376" t="s">
-        <v>5606</v>
+        <v>5607</v>
       </c>
       <c r="B376" t="s">
-        <v>1713</v>
+        <v>1714</v>
       </c>
       <c r="C376" t="s">
         <v>253</v>
@@ -49883,10 +49883,10 @@
     </row>
     <row r="377" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A377" t="s">
-        <v>5607</v>
+        <v>5608</v>
       </c>
       <c r="B377" t="s">
-        <v>1714</v>
+        <v>1715</v>
       </c>
       <c r="C377" t="s">
         <v>253</v>
@@ -49894,10 +49894,10 @@
     </row>
     <row r="378" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A378" t="s">
-        <v>5608</v>
+        <v>5609</v>
       </c>
       <c r="B378" t="s">
-        <v>1715</v>
+        <v>1716</v>
       </c>
       <c r="C378" t="s">
         <v>253</v>
@@ -49905,10 +49905,10 @@
     </row>
     <row r="379" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A379" t="s">
-        <v>5609</v>
+        <v>5610</v>
       </c>
       <c r="B379" t="s">
-        <v>1716</v>
+        <v>1717</v>
       </c>
       <c r="C379" t="s">
         <v>253</v>
@@ -49916,10 +49916,10 @@
     </row>
     <row r="380" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A380" t="s">
-        <v>5610</v>
+        <v>5612</v>
       </c>
       <c r="B380" t="s">
-        <v>1717</v>
+        <v>1719</v>
       </c>
       <c r="C380" t="s">
         <v>253</v>
@@ -49927,10 +49927,10 @@
     </row>
     <row r="381" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A381" t="s">
-        <v>5612</v>
+        <v>5613</v>
       </c>
       <c r="B381" t="s">
-        <v>1719</v>
+        <v>1720</v>
       </c>
       <c r="C381" t="s">
         <v>253</v>
@@ -49938,10 +49938,10 @@
     </row>
     <row r="382" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A382" t="s">
-        <v>5613</v>
+        <v>5614</v>
       </c>
       <c r="B382" t="s">
-        <v>1720</v>
+        <v>1721</v>
       </c>
       <c r="C382" t="s">
         <v>253</v>
@@ -49949,10 +49949,10 @@
     </row>
     <row r="383" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A383" t="s">
-        <v>5614</v>
+        <v>5615</v>
       </c>
       <c r="B383" t="s">
-        <v>1721</v>
+        <v>1722</v>
       </c>
       <c r="C383" t="s">
         <v>253</v>
@@ -49960,10 +49960,10 @@
     </row>
     <row r="384" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A384" t="s">
-        <v>5615</v>
+        <v>5616</v>
       </c>
       <c r="B384" t="s">
-        <v>1722</v>
+        <v>1723</v>
       </c>
       <c r="C384" t="s">
         <v>253</v>
@@ -49971,21 +49971,21 @@
     </row>
     <row r="385" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A385" t="s">
-        <v>5616</v>
+        <v>5617</v>
       </c>
       <c r="B385" t="s">
-        <v>1723</v>
+        <v>892</v>
       </c>
       <c r="C385" t="s">
-        <v>253</v>
+        <v>234</v>
       </c>
     </row>
     <row r="386" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A386" t="s">
-        <v>5617</v>
+        <v>5618</v>
       </c>
       <c r="B386" t="s">
-        <v>892</v>
+        <v>894</v>
       </c>
       <c r="C386" t="s">
         <v>234</v>
@@ -49993,10 +49993,10 @@
     </row>
     <row r="387" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A387" t="s">
-        <v>5618</v>
+        <v>5619</v>
       </c>
       <c r="B387" t="s">
-        <v>894</v>
+        <v>895</v>
       </c>
       <c r="C387" t="s">
         <v>234</v>
@@ -50004,98 +50004,98 @@
     </row>
     <row r="388" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A388" t="s">
-        <v>5619</v>
+        <v>5620</v>
       </c>
       <c r="B388" t="s">
-        <v>895</v>
+        <v>889</v>
       </c>
       <c r="C388" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="389" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A389" t="s">
-        <v>5620</v>
+        <v>5621</v>
       </c>
       <c r="B389" t="s">
-        <v>889</v>
+        <v>891</v>
       </c>
       <c r="C389" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
     </row>
     <row r="390" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A390" t="s">
-        <v>5621</v>
+        <v>5622</v>
       </c>
       <c r="B390" t="s">
-        <v>891</v>
+        <v>902</v>
       </c>
       <c r="C390" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
     </row>
     <row r="391" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A391" t="s">
-        <v>5622</v>
+        <v>5623</v>
       </c>
       <c r="B391" t="s">
-        <v>902</v>
+        <v>890</v>
       </c>
       <c r="C391" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
     </row>
     <row r="392" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A392" t="s">
-        <v>5623</v>
+        <v>5624</v>
       </c>
       <c r="B392" t="s">
-        <v>890</v>
+        <v>893</v>
       </c>
       <c r="C392" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
     </row>
     <row r="393" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A393" t="s">
-        <v>5624</v>
+        <v>5625</v>
       </c>
       <c r="B393" t="s">
-        <v>893</v>
+        <v>898</v>
       </c>
       <c r="C393" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
     </row>
     <row r="394" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A394" t="s">
-        <v>5625</v>
+        <v>5626</v>
       </c>
       <c r="B394" t="s">
-        <v>898</v>
+        <v>1156</v>
       </c>
       <c r="C394" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
     </row>
     <row r="395" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A395" t="s">
-        <v>5626</v>
+        <v>5627</v>
       </c>
       <c r="B395" t="s">
-        <v>1156</v>
+        <v>899</v>
       </c>
       <c r="C395" t="s">
-        <v>253</v>
+        <v>232</v>
       </c>
     </row>
     <row r="396" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A396" t="s">
-        <v>5627</v>
+        <v>5628</v>
       </c>
       <c r="B396" t="s">
-        <v>899</v>
+        <v>896</v>
       </c>
       <c r="C396" t="s">
         <v>232</v>
@@ -50103,54 +50103,54 @@
     </row>
     <row r="397" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A397" t="s">
-        <v>5628</v>
+        <v>5629</v>
       </c>
       <c r="B397" t="s">
-        <v>896</v>
+        <v>897</v>
       </c>
       <c r="C397" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
     </row>
     <row r="398" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A398" t="s">
-        <v>5629</v>
+        <v>5630</v>
       </c>
       <c r="B398" t="s">
-        <v>897</v>
+        <v>901</v>
       </c>
       <c r="C398" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
     </row>
     <row r="399" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A399" t="s">
-        <v>5630</v>
+        <v>5631</v>
       </c>
       <c r="B399" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="C399" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="400" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A400" t="s">
-        <v>5631</v>
+        <v>5632</v>
       </c>
       <c r="B400" t="s">
-        <v>900</v>
+        <v>906</v>
       </c>
       <c r="C400" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
     </row>
     <row r="401" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A401" t="s">
-        <v>5632</v>
+        <v>5633</v>
       </c>
       <c r="B401" t="s">
-        <v>906</v>
+        <v>903</v>
       </c>
       <c r="C401" t="s">
         <v>238</v>
@@ -50158,10 +50158,10 @@
     </row>
     <row r="402" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A402" t="s">
-        <v>5633</v>
+        <v>5634</v>
       </c>
       <c r="B402" t="s">
-        <v>903</v>
+        <v>905</v>
       </c>
       <c r="C402" t="s">
         <v>238</v>
@@ -50169,10 +50169,10 @@
     </row>
     <row r="403" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A403" t="s">
-        <v>5634</v>
+        <v>5635</v>
       </c>
       <c r="B403" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="C403" t="s">
         <v>238</v>
@@ -50180,54 +50180,54 @@
     </row>
     <row r="404" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A404" t="s">
-        <v>5635</v>
+        <v>5636</v>
       </c>
       <c r="B404" t="s">
-        <v>904</v>
+        <v>914</v>
       </c>
       <c r="C404" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="405" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A405" t="s">
-        <v>5636</v>
+        <v>5637</v>
       </c>
       <c r="B405" t="s">
-        <v>914</v>
+        <v>911</v>
       </c>
       <c r="C405" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
     </row>
     <row r="406" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A406" t="s">
-        <v>5637</v>
+        <v>5638</v>
       </c>
       <c r="B406" t="s">
-        <v>911</v>
+        <v>877</v>
       </c>
       <c r="C406" t="s">
-        <v>240</v>
+        <v>253</v>
       </c>
     </row>
     <row r="407" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A407" t="s">
-        <v>5638</v>
+        <v>5639</v>
       </c>
       <c r="B407" t="s">
-        <v>877</v>
+        <v>912</v>
       </c>
       <c r="C407" t="s">
-        <v>253</v>
+        <v>240</v>
       </c>
     </row>
     <row r="408" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A408" t="s">
-        <v>5639</v>
+        <v>5640</v>
       </c>
       <c r="B408" t="s">
-        <v>912</v>
+        <v>907</v>
       </c>
       <c r="C408" t="s">
         <v>240</v>
@@ -50235,21 +50235,21 @@
     </row>
     <row r="409" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A409" t="s">
-        <v>5640</v>
+        <v>5641</v>
       </c>
       <c r="B409" t="s">
-        <v>907</v>
+        <v>876</v>
       </c>
       <c r="C409" t="s">
-        <v>240</v>
+        <v>253</v>
       </c>
     </row>
     <row r="410" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A410" t="s">
-        <v>5641</v>
+        <v>5642</v>
       </c>
       <c r="B410" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
       <c r="C410" t="s">
         <v>253</v>
@@ -50257,21 +50257,21 @@
     </row>
     <row r="411" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A411" t="s">
-        <v>5642</v>
+        <v>5643</v>
       </c>
       <c r="B411" t="s">
-        <v>874</v>
+        <v>910</v>
       </c>
       <c r="C411" t="s">
-        <v>253</v>
+        <v>240</v>
       </c>
     </row>
     <row r="412" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A412" t="s">
-        <v>5643</v>
+        <v>5644</v>
       </c>
       <c r="B412" t="s">
-        <v>910</v>
+        <v>916</v>
       </c>
       <c r="C412" t="s">
         <v>240</v>
@@ -50279,43 +50279,43 @@
     </row>
     <row r="413" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A413" t="s">
-        <v>5644</v>
+        <v>5645</v>
       </c>
       <c r="B413" t="s">
-        <v>916</v>
+        <v>917</v>
       </c>
       <c r="C413" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
     </row>
     <row r="414" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A414" t="s">
-        <v>5645</v>
+        <v>5646</v>
       </c>
       <c r="B414" t="s">
-        <v>917</v>
+        <v>918</v>
       </c>
       <c r="C414" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="415" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A415" t="s">
-        <v>5646</v>
+        <v>5647</v>
       </c>
       <c r="B415" t="s">
-        <v>918</v>
+        <v>915</v>
       </c>
       <c r="C415" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
     </row>
     <row r="416" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A416" t="s">
-        <v>5647</v>
+        <v>5648</v>
       </c>
       <c r="B416" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="C416" t="s">
         <v>236</v>
@@ -50323,10 +50323,10 @@
     </row>
     <row r="417" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A417" t="s">
-        <v>5648</v>
+        <v>5649</v>
       </c>
       <c r="B417" t="s">
-        <v>913</v>
+        <v>919</v>
       </c>
       <c r="C417" t="s">
         <v>236</v>
@@ -50334,21 +50334,21 @@
     </row>
     <row r="418" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A418" t="s">
-        <v>5649</v>
+        <v>5650</v>
       </c>
       <c r="B418" t="s">
-        <v>919</v>
+        <v>908</v>
       </c>
       <c r="C418" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
     </row>
     <row r="419" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A419" t="s">
-        <v>5650</v>
+        <v>5651</v>
       </c>
       <c r="B419" t="s">
-        <v>908</v>
+        <v>909</v>
       </c>
       <c r="C419" t="s">
         <v>240</v>
@@ -50356,54 +50356,54 @@
     </row>
     <row r="420" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A420" t="s">
-        <v>5651</v>
+        <v>5652</v>
       </c>
       <c r="B420" t="s">
-        <v>909</v>
+        <v>1812</v>
       </c>
       <c r="C420" t="s">
-        <v>240</v>
+        <v>331</v>
       </c>
     </row>
     <row r="421" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A421" t="s">
-        <v>5652</v>
+        <v>5653</v>
       </c>
       <c r="B421" t="s">
-        <v>1812</v>
+        <v>855</v>
       </c>
       <c r="C421" t="s">
-        <v>331</v>
+        <v>147</v>
       </c>
     </row>
     <row r="422" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A422" t="s">
-        <v>5653</v>
+        <v>5654</v>
       </c>
       <c r="B422" t="s">
-        <v>855</v>
+        <v>4507</v>
       </c>
       <c r="C422" t="s">
-        <v>147</v>
+        <v>170</v>
       </c>
     </row>
     <row r="423" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A423" t="s">
-        <v>5654</v>
+        <v>5809</v>
       </c>
       <c r="B423" t="s">
-        <v>4507</v>
+        <v>5810</v>
       </c>
       <c r="C423" t="s">
-        <v>170</v>
+        <v>243</v>
       </c>
     </row>
     <row r="424" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A424" t="s">
-        <v>5809</v>
+        <v>5655</v>
       </c>
       <c r="B424" t="s">
-        <v>5810</v>
+        <v>856</v>
       </c>
       <c r="C424" t="s">
         <v>243</v>
@@ -50411,10 +50411,10 @@
     </row>
     <row r="425" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A425" t="s">
-        <v>5655</v>
+        <v>5656</v>
       </c>
       <c r="B425" t="s">
-        <v>856</v>
+        <v>857</v>
       </c>
       <c r="C425" t="s">
         <v>243</v>
@@ -50422,10 +50422,10 @@
     </row>
     <row r="426" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A426" t="s">
-        <v>5656</v>
+        <v>5811</v>
       </c>
       <c r="B426" t="s">
-        <v>857</v>
+        <v>5812</v>
       </c>
       <c r="C426" t="s">
         <v>243</v>
@@ -50433,10 +50433,10 @@
     </row>
     <row r="427" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A427" t="s">
-        <v>5811</v>
+        <v>5657</v>
       </c>
       <c r="B427" t="s">
-        <v>5812</v>
+        <v>2547</v>
       </c>
       <c r="C427" t="s">
         <v>243</v>
@@ -50444,32 +50444,32 @@
     </row>
     <row r="428" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A428" t="s">
-        <v>5657</v>
+        <v>5658</v>
       </c>
       <c r="B428" t="s">
-        <v>2547</v>
+        <v>920</v>
       </c>
       <c r="C428" t="s">
-        <v>243</v>
+        <v>251</v>
       </c>
     </row>
     <row r="429" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A429" t="s">
-        <v>5658</v>
+        <v>5659</v>
       </c>
       <c r="B429" t="s">
-        <v>920</v>
+        <v>4508</v>
       </c>
       <c r="C429" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
     </row>
     <row r="430" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A430" t="s">
-        <v>5659</v>
+        <v>5660</v>
       </c>
       <c r="B430" t="s">
-        <v>4508</v>
+        <v>4509</v>
       </c>
       <c r="C430" t="s">
         <v>243</v>
@@ -50477,10 +50477,10 @@
     </row>
     <row r="431" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A431" t="s">
-        <v>5660</v>
+        <v>5661</v>
       </c>
       <c r="B431" t="s">
-        <v>4509</v>
+        <v>4510</v>
       </c>
       <c r="C431" t="s">
         <v>243</v>
@@ -50488,10 +50488,10 @@
     </row>
     <row r="432" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A432" t="s">
-        <v>5661</v>
+        <v>5662</v>
       </c>
       <c r="B432" t="s">
-        <v>4510</v>
+        <v>4511</v>
       </c>
       <c r="C432" t="s">
         <v>243</v>
@@ -50499,21 +50499,21 @@
     </row>
     <row r="433" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A433" t="s">
-        <v>5662</v>
+        <v>5663</v>
       </c>
       <c r="B433" t="s">
-        <v>4511</v>
+        <v>4512</v>
       </c>
       <c r="C433" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
     </row>
     <row r="434" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A434" t="s">
-        <v>5663</v>
+        <v>5664</v>
       </c>
       <c r="B434" t="s">
-        <v>4512</v>
+        <v>4513</v>
       </c>
       <c r="C434" t="s">
         <v>234</v>
@@ -50521,10 +50521,10 @@
     </row>
     <row r="435" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A435" t="s">
-        <v>5664</v>
+        <v>5665</v>
       </c>
       <c r="B435" t="s">
-        <v>4513</v>
+        <v>4514</v>
       </c>
       <c r="C435" t="s">
         <v>234</v>
@@ -50532,10 +50532,10 @@
     </row>
     <row r="436" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A436" t="s">
-        <v>5665</v>
+        <v>5666</v>
       </c>
       <c r="B436" t="s">
-        <v>4514</v>
+        <v>4515</v>
       </c>
       <c r="C436" t="s">
         <v>234</v>
@@ -50543,21 +50543,21 @@
     </row>
     <row r="437" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A437" t="s">
-        <v>5666</v>
+        <v>5667</v>
       </c>
       <c r="B437" t="s">
-        <v>4515</v>
+        <v>4516</v>
       </c>
       <c r="C437" t="s">
-        <v>234</v>
+        <v>243</v>
       </c>
     </row>
     <row r="438" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A438" t="s">
-        <v>5667</v>
+        <v>5668</v>
       </c>
       <c r="B438" t="s">
-        <v>4516</v>
+        <v>4517</v>
       </c>
       <c r="C438" t="s">
         <v>243</v>
@@ -50565,21 +50565,21 @@
     </row>
     <row r="439" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A439" t="s">
-        <v>5668</v>
+        <v>5669</v>
       </c>
       <c r="B439" t="s">
-        <v>4517</v>
+        <v>4518</v>
       </c>
       <c r="C439" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
     </row>
     <row r="440" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A440" t="s">
-        <v>5669</v>
+        <v>5670</v>
       </c>
       <c r="B440" t="s">
-        <v>4518</v>
+        <v>4519</v>
       </c>
       <c r="C440" t="s">
         <v>234</v>
@@ -50587,10 +50587,10 @@
     </row>
     <row r="441" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A441" t="s">
-        <v>5670</v>
+        <v>5671</v>
       </c>
       <c r="B441" t="s">
-        <v>4519</v>
+        <v>4520</v>
       </c>
       <c r="C441" t="s">
         <v>234</v>
@@ -50598,32 +50598,32 @@
     </row>
     <row r="442" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A442" t="s">
-        <v>5671</v>
+        <v>5672</v>
       </c>
       <c r="B442" t="s">
-        <v>4520</v>
+        <v>4521</v>
       </c>
       <c r="C442" t="s">
-        <v>234</v>
+        <v>243</v>
       </c>
     </row>
     <row r="443" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A443" t="s">
-        <v>5672</v>
+        <v>5673</v>
       </c>
       <c r="B443" t="s">
-        <v>4521</v>
+        <v>1065</v>
       </c>
       <c r="C443" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
     </row>
     <row r="444" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A444" t="s">
-        <v>5673</v>
+        <v>5674</v>
       </c>
       <c r="B444" t="s">
-        <v>1065</v>
+        <v>1070</v>
       </c>
       <c r="C444" t="s">
         <v>234</v>
@@ -50631,10 +50631,10 @@
     </row>
     <row r="445" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A445" t="s">
-        <v>5674</v>
+        <v>5675</v>
       </c>
       <c r="B445" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="C445" t="s">
         <v>234</v>
@@ -50642,10 +50642,10 @@
     </row>
     <row r="446" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A446" t="s">
-        <v>5675</v>
+        <v>5676</v>
       </c>
       <c r="B446" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="C446" t="s">
         <v>234</v>
@@ -50653,10 +50653,10 @@
     </row>
     <row r="447" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A447" t="s">
-        <v>5676</v>
+        <v>5677</v>
       </c>
       <c r="B447" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="C447" t="s">
         <v>234</v>
@@ -50664,10 +50664,10 @@
     </row>
     <row r="448" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A448" t="s">
-        <v>5677</v>
+        <v>5678</v>
       </c>
       <c r="B448" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="C448" t="s">
         <v>234</v>
@@ -50675,54 +50675,54 @@
     </row>
     <row r="449" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A449" t="s">
-        <v>5678</v>
+        <v>5486</v>
       </c>
       <c r="B449" t="s">
-        <v>1066</v>
+        <v>1008</v>
       </c>
       <c r="C449" t="s">
-        <v>234</v>
+        <v>334</v>
       </c>
     </row>
     <row r="450" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A450" t="s">
-        <v>5486</v>
+        <v>5215</v>
       </c>
       <c r="B450" t="s">
-        <v>1008</v>
+        <v>969</v>
       </c>
       <c r="C450" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="451" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A451" t="s">
-        <v>5215</v>
+        <v>5679</v>
       </c>
       <c r="B451" t="s">
-        <v>969</v>
+        <v>1076</v>
       </c>
       <c r="C451" t="s">
-        <v>332</v>
+        <v>345</v>
       </c>
     </row>
     <row r="452" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A452" t="s">
-        <v>5679</v>
+        <v>5680</v>
       </c>
       <c r="B452" t="s">
-        <v>1076</v>
+        <v>4530</v>
       </c>
       <c r="C452" t="s">
-        <v>345</v>
+        <v>242</v>
       </c>
     </row>
     <row r="453" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A453" t="s">
-        <v>5680</v>
+        <v>5681</v>
       </c>
       <c r="B453" t="s">
-        <v>4530</v>
+        <v>4531</v>
       </c>
       <c r="C453" t="s">
         <v>242</v>
@@ -50730,10 +50730,10 @@
     </row>
     <row r="454" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A454" t="s">
-        <v>5681</v>
+        <v>5682</v>
       </c>
       <c r="B454" t="s">
-        <v>4531</v>
+        <v>4532</v>
       </c>
       <c r="C454" t="s">
         <v>242</v>
@@ -50741,10 +50741,10 @@
     </row>
     <row r="455" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A455" t="s">
-        <v>5682</v>
+        <v>5683</v>
       </c>
       <c r="B455" t="s">
-        <v>4532</v>
+        <v>4533</v>
       </c>
       <c r="C455" t="s">
         <v>242</v>
@@ -50752,10 +50752,10 @@
     </row>
     <row r="456" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A456" t="s">
-        <v>5683</v>
+        <v>5684</v>
       </c>
       <c r="B456" t="s">
-        <v>4533</v>
+        <v>4534</v>
       </c>
       <c r="C456" t="s">
         <v>242</v>
@@ -50763,10 +50763,10 @@
     </row>
     <row r="457" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A457" t="s">
-        <v>5684</v>
+        <v>5685</v>
       </c>
       <c r="B457" t="s">
-        <v>4534</v>
+        <v>4535</v>
       </c>
       <c r="C457" t="s">
         <v>242</v>
@@ -50774,10 +50774,10 @@
     </row>
     <row r="458" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A458" t="s">
-        <v>5685</v>
+        <v>5686</v>
       </c>
       <c r="B458" t="s">
-        <v>4535</v>
+        <v>4536</v>
       </c>
       <c r="C458" t="s">
         <v>242</v>
@@ -50785,10 +50785,10 @@
     </row>
     <row r="459" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A459" t="s">
-        <v>5686</v>
+        <v>5687</v>
       </c>
       <c r="B459" t="s">
-        <v>4536</v>
+        <v>4537</v>
       </c>
       <c r="C459" t="s">
         <v>242</v>
@@ -50796,10 +50796,10 @@
     </row>
     <row r="460" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A460" t="s">
-        <v>5687</v>
+        <v>5688</v>
       </c>
       <c r="B460" t="s">
-        <v>4537</v>
+        <v>4538</v>
       </c>
       <c r="C460" t="s">
         <v>242</v>
@@ -50807,10 +50807,10 @@
     </row>
     <row r="461" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A461" t="s">
-        <v>5688</v>
+        <v>5689</v>
       </c>
       <c r="B461" t="s">
-        <v>4538</v>
+        <v>4539</v>
       </c>
       <c r="C461" t="s">
         <v>242</v>
@@ -50818,10 +50818,10 @@
     </row>
     <row r="462" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A462" t="s">
-        <v>5689</v>
+        <v>5690</v>
       </c>
       <c r="B462" t="s">
-        <v>4539</v>
+        <v>4540</v>
       </c>
       <c r="C462" t="s">
         <v>242</v>
@@ -50829,10 +50829,10 @@
     </row>
     <row r="463" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A463" t="s">
-        <v>5690</v>
+        <v>5691</v>
       </c>
       <c r="B463" t="s">
-        <v>4540</v>
+        <v>4541</v>
       </c>
       <c r="C463" t="s">
         <v>242</v>
@@ -50840,10 +50840,10 @@
     </row>
     <row r="464" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A464" t="s">
-        <v>5691</v>
+        <v>5692</v>
       </c>
       <c r="B464" t="s">
-        <v>4541</v>
+        <v>4542</v>
       </c>
       <c r="C464" t="s">
         <v>242</v>
@@ -50851,21 +50851,21 @@
     </row>
     <row r="465" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A465" t="s">
-        <v>5692</v>
+        <v>5693</v>
       </c>
       <c r="B465" t="s">
-        <v>4542</v>
+        <v>4543</v>
       </c>
       <c r="C465" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
     </row>
     <row r="466" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A466" t="s">
-        <v>5693</v>
+        <v>5694</v>
       </c>
       <c r="B466" t="s">
-        <v>4543</v>
+        <v>4544</v>
       </c>
       <c r="C466" t="s">
         <v>245</v>
@@ -50873,10 +50873,10 @@
     </row>
     <row r="467" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A467" t="s">
-        <v>5694</v>
+        <v>5695</v>
       </c>
       <c r="B467" t="s">
-        <v>4544</v>
+        <v>4545</v>
       </c>
       <c r="C467" t="s">
         <v>245</v>
@@ -50884,10 +50884,10 @@
     </row>
     <row r="468" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A468" t="s">
-        <v>5695</v>
+        <v>5696</v>
       </c>
       <c r="B468" t="s">
-        <v>4545</v>
+        <v>4546</v>
       </c>
       <c r="C468" t="s">
         <v>245</v>
@@ -50895,10 +50895,10 @@
     </row>
     <row r="469" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A469" t="s">
-        <v>5696</v>
+        <v>5697</v>
       </c>
       <c r="B469" t="s">
-        <v>4546</v>
+        <v>4547</v>
       </c>
       <c r="C469" t="s">
         <v>245</v>
@@ -50906,10 +50906,10 @@
     </row>
     <row r="470" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A470" t="s">
-        <v>5697</v>
+        <v>5698</v>
       </c>
       <c r="B470" t="s">
-        <v>4547</v>
+        <v>4548</v>
       </c>
       <c r="C470" t="s">
         <v>245</v>
@@ -50917,10 +50917,10 @@
     </row>
     <row r="471" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A471" t="s">
-        <v>5698</v>
+        <v>5699</v>
       </c>
       <c r="B471" t="s">
-        <v>4548</v>
+        <v>4549</v>
       </c>
       <c r="C471" t="s">
         <v>245</v>
@@ -50928,10 +50928,10 @@
     </row>
     <row r="472" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A472" t="s">
-        <v>5699</v>
+        <v>5700</v>
       </c>
       <c r="B472" t="s">
-        <v>4549</v>
+        <v>4550</v>
       </c>
       <c r="C472" t="s">
         <v>245</v>
@@ -50939,10 +50939,10 @@
     </row>
     <row r="473" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A473" t="s">
-        <v>5700</v>
+        <v>5701</v>
       </c>
       <c r="B473" t="s">
-        <v>4550</v>
+        <v>4551</v>
       </c>
       <c r="C473" t="s">
         <v>245</v>
@@ -50950,10 +50950,10 @@
     </row>
     <row r="474" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A474" t="s">
-        <v>5701</v>
+        <v>5702</v>
       </c>
       <c r="B474" t="s">
-        <v>4551</v>
+        <v>4552</v>
       </c>
       <c r="C474" t="s">
         <v>245</v>
@@ -50961,10 +50961,10 @@
     </row>
     <row r="475" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A475" t="s">
-        <v>5702</v>
+        <v>5703</v>
       </c>
       <c r="B475" t="s">
-        <v>4552</v>
+        <v>4553</v>
       </c>
       <c r="C475" t="s">
         <v>245</v>
@@ -50972,10 +50972,10 @@
     </row>
     <row r="476" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A476" t="s">
-        <v>5703</v>
+        <v>5704</v>
       </c>
       <c r="B476" t="s">
-        <v>4553</v>
+        <v>4554</v>
       </c>
       <c r="C476" t="s">
         <v>245</v>
@@ -50983,10 +50983,10 @@
     </row>
     <row r="477" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A477" t="s">
-        <v>5704</v>
+        <v>5705</v>
       </c>
       <c r="B477" t="s">
-        <v>4554</v>
+        <v>4555</v>
       </c>
       <c r="C477" t="s">
         <v>245</v>
@@ -50994,10 +50994,10 @@
     </row>
     <row r="478" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A478" t="s">
-        <v>5705</v>
+        <v>5706</v>
       </c>
       <c r="B478" t="s">
-        <v>4555</v>
+        <v>4556</v>
       </c>
       <c r="C478" t="s">
         <v>245</v>
@@ -51005,10 +51005,10 @@
     </row>
     <row r="479" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A479" t="s">
-        <v>5706</v>
+        <v>5707</v>
       </c>
       <c r="B479" t="s">
-        <v>4556</v>
+        <v>4557</v>
       </c>
       <c r="C479" t="s">
         <v>245</v>
@@ -51016,10 +51016,10 @@
     </row>
     <row r="480" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A480" t="s">
-        <v>5707</v>
+        <v>5708</v>
       </c>
       <c r="B480" t="s">
-        <v>4557</v>
+        <v>4558</v>
       </c>
       <c r="C480" t="s">
         <v>245</v>
@@ -51027,10 +51027,10 @@
     </row>
     <row r="481" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A481" t="s">
-        <v>5708</v>
+        <v>5709</v>
       </c>
       <c r="B481" t="s">
-        <v>4558</v>
+        <v>4559</v>
       </c>
       <c r="C481" t="s">
         <v>245</v>
@@ -51038,10 +51038,10 @@
     </row>
     <row r="482" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A482" t="s">
-        <v>5709</v>
+        <v>5710</v>
       </c>
       <c r="B482" t="s">
-        <v>4559</v>
+        <v>4560</v>
       </c>
       <c r="C482" t="s">
         <v>245</v>
@@ -51049,21 +51049,21 @@
     </row>
     <row r="483" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A483" t="s">
-        <v>5710</v>
+        <v>5711</v>
       </c>
       <c r="B483" t="s">
-        <v>4560</v>
+        <v>4596</v>
       </c>
       <c r="C483" t="s">
-        <v>245</v>
+        <v>326</v>
       </c>
     </row>
     <row r="484" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A484" t="s">
-        <v>5711</v>
+        <v>5712</v>
       </c>
       <c r="B484" t="s">
-        <v>4596</v>
+        <v>4597</v>
       </c>
       <c r="C484" t="s">
         <v>326</v>
@@ -51071,32 +51071,32 @@
     </row>
     <row r="485" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A485" t="s">
-        <v>5712</v>
+        <v>5713</v>
       </c>
       <c r="B485" t="s">
-        <v>4597</v>
+        <v>2169</v>
       </c>
       <c r="C485" t="s">
-        <v>326</v>
+        <v>170</v>
       </c>
     </row>
     <row r="486" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A486" t="s">
-        <v>5713</v>
+        <v>5714</v>
       </c>
       <c r="B486" t="s">
-        <v>2169</v>
+        <v>858</v>
       </c>
       <c r="C486" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="487" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A487" t="s">
-        <v>5714</v>
+        <v>5715</v>
       </c>
       <c r="B487" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="C487" t="s">
         <v>168</v>
@@ -51104,10 +51104,10 @@
     </row>
     <row r="488" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A488" t="s">
-        <v>5715</v>
+        <v>5716</v>
       </c>
       <c r="B488" t="s">
-        <v>859</v>
+        <v>861</v>
       </c>
       <c r="C488" t="s">
         <v>168</v>
@@ -51115,10 +51115,10 @@
     </row>
     <row r="489" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A489" t="s">
-        <v>5716</v>
+        <v>5717</v>
       </c>
       <c r="B489" t="s">
-        <v>861</v>
+        <v>863</v>
       </c>
       <c r="C489" t="s">
         <v>168</v>
@@ -51126,10 +51126,10 @@
     </row>
     <row r="490" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A490" t="s">
-        <v>5717</v>
+        <v>5718</v>
       </c>
       <c r="B490" t="s">
-        <v>863</v>
+        <v>864</v>
       </c>
       <c r="C490" t="s">
         <v>168</v>
@@ -51137,21 +51137,21 @@
     </row>
     <row r="491" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A491" t="s">
-        <v>5718</v>
+        <v>5719</v>
       </c>
       <c r="B491" t="s">
-        <v>864</v>
+        <v>4956</v>
       </c>
       <c r="C491" t="s">
-        <v>168</v>
+        <v>316</v>
       </c>
     </row>
     <row r="492" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A492" t="s">
-        <v>5719</v>
+        <v>5720</v>
       </c>
       <c r="B492" t="s">
-        <v>4956</v>
+        <v>4957</v>
       </c>
       <c r="C492" t="s">
         <v>316</v>
@@ -51159,21 +51159,21 @@
     </row>
     <row r="493" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A493" t="s">
-        <v>5720</v>
+        <v>5721</v>
       </c>
       <c r="B493" t="s">
-        <v>4957</v>
+        <v>860</v>
       </c>
       <c r="C493" t="s">
-        <v>316</v>
+        <v>166</v>
       </c>
     </row>
     <row r="494" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A494" t="s">
-        <v>5721</v>
+        <v>5722</v>
       </c>
       <c r="B494" t="s">
-        <v>860</v>
+        <v>862</v>
       </c>
       <c r="C494" t="s">
         <v>166</v>
@@ -51181,54 +51181,54 @@
     </row>
     <row r="495" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A495" t="s">
-        <v>5722</v>
+        <v>5813</v>
       </c>
       <c r="B495" t="s">
-        <v>862</v>
+        <v>5814</v>
       </c>
       <c r="C495" t="s">
-        <v>166</v>
+        <v>197</v>
       </c>
     </row>
     <row r="496" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A496" t="s">
-        <v>5813</v>
+        <v>5723</v>
       </c>
       <c r="B496" t="s">
-        <v>5814</v>
+        <v>865</v>
       </c>
       <c r="C496" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="497" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A497" t="s">
-        <v>5723</v>
+        <v>5724</v>
       </c>
       <c r="B497" t="s">
-        <v>865</v>
+        <v>5091</v>
       </c>
       <c r="C497" t="s">
-        <v>199</v>
+        <v>243</v>
       </c>
     </row>
     <row r="498" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A498" t="s">
-        <v>5724</v>
+        <v>5725</v>
       </c>
       <c r="B498" t="s">
-        <v>5091</v>
+        <v>5092</v>
       </c>
       <c r="C498" t="s">
-        <v>243</v>
+        <v>232</v>
       </c>
     </row>
     <row r="499" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A499" t="s">
-        <v>5725</v>
+        <v>5726</v>
       </c>
       <c r="B499" t="s">
-        <v>5092</v>
+        <v>5093</v>
       </c>
       <c r="C499" t="s">
         <v>232</v>
@@ -51236,21 +51236,21 @@
     </row>
     <row r="500" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A500" t="s">
-        <v>5726</v>
+        <v>5727</v>
       </c>
       <c r="B500" t="s">
-        <v>5093</v>
+        <v>5094</v>
       </c>
       <c r="C500" t="s">
-        <v>232</v>
+        <v>245</v>
       </c>
     </row>
     <row r="501" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A501" t="s">
-        <v>5727</v>
+        <v>5728</v>
       </c>
       <c r="B501" t="s">
-        <v>5094</v>
+        <v>5095</v>
       </c>
       <c r="C501" t="s">
         <v>245</v>
@@ -51258,10 +51258,10 @@
     </row>
     <row r="502" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A502" t="s">
-        <v>5728</v>
+        <v>5729</v>
       </c>
       <c r="B502" t="s">
-        <v>5095</v>
+        <v>5096</v>
       </c>
       <c r="C502" t="s">
         <v>245</v>
@@ -51269,45 +51269,34 @@
     </row>
     <row r="503" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A503" t="s">
-        <v>5729</v>
+        <v>5730</v>
       </c>
       <c r="B503" t="s">
-        <v>5096</v>
+        <v>5097</v>
       </c>
       <c r="C503" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="504" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A504" t="s">
-        <v>5730</v>
+        <v>5731</v>
       </c>
       <c r="B504" t="s">
-        <v>5097</v>
+        <v>5098</v>
       </c>
       <c r="C504" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="505" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A505" t="s">
-        <v>5731</v>
+        <v>5732</v>
       </c>
       <c r="B505" t="s">
-        <v>5098</v>
+        <v>2957</v>
       </c>
       <c r="C505" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="506" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A506" t="s">
-        <v>5732</v>
-      </c>
-      <c r="B506" t="s">
-        <v>2957</v>
-      </c>
-      <c r="C506" t="s">
         <v>337</v>
       </c>
     </row>

</xml_diff>